<commit_message>
update logs, research and add laser cutting files
</commit_message>
<xml_diff>
--- a/Research/phone poll.xlsx
+++ b/Research/phone poll.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SujayGarlanka/Projects/Jamak.ai/Research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SujayGarlanka/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21560" windowHeight="14280" tabRatio="500"/>
+    <workbookView xWindow="4660" yWindow="460" windowWidth="16280" windowHeight="14280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -152,7 +152,7 @@
     <t>Vivo Y12s</t>
   </si>
   <si>
-    <t>USB USB Type-C 3.1, USB On-The-Go</t>
+    <t>USB Type-C 3.1, USB On-The-Go</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>